<commit_message>
Improved code, added comments and markdowns, added PPG statistic, added table of last game (with user interactivity allowing to select another game)
</commit_message>
<xml_diff>
--- a/Poker League 2023.xlsx
+++ b/Poker League 2023.xlsx
@@ -5,17 +5,18 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PanSt\OneDrive\Υπολογιστής\Poker-League-Game-Analysis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/89771c8abd0f3387/Υπολογιστής/Poker-League-Game-Analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5806CCF-3535-4441-AFC9-197C84631A5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{304CEC61-5BD2-4202-9E7B-2C5AE805189D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Φύλλο1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -483,22 +484,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AG34"/>
+  <dimension ref="A1:AH34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="105" zoomScaleNormal="145" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="Q26" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AG35" sqref="AG35"/>
+      <selection pane="bottomRight" activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="8.88671875" style="3"/>
-    <col min="3" max="3" width="8.88671875" style="2"/>
+    <col min="2" max="2" width="8.85546875" style="3"/>
+    <col min="3" max="3" width="8.85546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:34" x14ac:dyDescent="0.25">
       <c r="B1" s="3" t="s">
         <v>7</v>
       </c>
@@ -595,22 +596,25 @@
       <c r="AG1" s="1">
         <v>45239</v>
       </c>
-    </row>
-    <row r="2" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="AH1" s="1">
+        <v>45244</v>
+      </c>
+    </row>
+    <row r="2" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="4">
-        <f t="shared" ref="B2:B33" si="0">SUM(E2:XFD2)</f>
-        <v>73.600000000000009</v>
+        <f t="shared" ref="B2:B34" si="0">SUM(E2:XFD2)</f>
+        <v>100.85000000000001</v>
       </c>
       <c r="C2" s="5">
-        <f t="shared" ref="C2:C33" si="1">B2/COUNT(E2:XFD2)</f>
-        <v>2.5379310344827588</v>
+        <f t="shared" ref="C2:C34" si="1">B2/COUNT(E2:XFD2)</f>
+        <v>3.3616666666666668</v>
       </c>
       <c r="D2">
-        <f t="shared" ref="D2:D33" si="2">COUNT(E2:XFD2)</f>
-        <v>29</v>
+        <f t="shared" ref="D2:D34" si="2">COUNT(E2:XFD2)</f>
+        <v>30</v>
       </c>
       <c r="E2">
         <v>-5</v>
@@ -699,22 +703,25 @@
       <c r="AG2">
         <v>-35</v>
       </c>
-    </row>
-    <row r="3" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="AH2">
+        <v>27.25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B3" s="4">
         <f t="shared" si="0"/>
-        <v>143.14999999999998</v>
+        <v>148.04999999999998</v>
       </c>
       <c r="C3" s="5">
         <f t="shared" si="1"/>
-        <v>5.3018518518518514</v>
+        <v>5.2874999999999996</v>
       </c>
       <c r="D3">
         <f t="shared" si="2"/>
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E3">
         <v>-15</v>
@@ -797,22 +804,25 @@
       <c r="AG3">
         <v>16.600000000000001</v>
       </c>
-    </row>
-    <row r="4" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="AH3">
+        <v>4.9000000000000004</v>
+      </c>
+    </row>
+    <row r="4" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B4" s="4">
         <f t="shared" si="0"/>
-        <v>109.39999999999999</v>
+        <v>103.80999999999999</v>
       </c>
       <c r="C4" s="5">
         <f t="shared" si="1"/>
-        <v>4.0518518518518514</v>
+        <v>3.7074999999999996</v>
       </c>
       <c r="D4">
         <f t="shared" si="2"/>
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E4">
         <v>-0.95</v>
@@ -895,22 +905,25 @@
       <c r="AG4">
         <v>-0.35</v>
       </c>
-    </row>
-    <row r="5" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="AH4">
+        <v>-5.59</v>
+      </c>
+    </row>
+    <row r="5" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B5" s="4">
         <f t="shared" si="0"/>
-        <v>77.699999999999989</v>
+        <v>57.699999999999989</v>
       </c>
       <c r="C5" s="5">
         <f t="shared" si="1"/>
-        <v>2.8777777777777773</v>
+        <v>2.0607142857142855</v>
       </c>
       <c r="D5">
         <f t="shared" si="2"/>
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E5">
         <v>37.35</v>
@@ -993,22 +1006,25 @@
       <c r="AG5">
         <v>-18.25</v>
       </c>
-    </row>
-    <row r="6" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="AH5">
+        <v>-20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B6" s="4">
         <f t="shared" si="0"/>
-        <v>166.95</v>
+        <v>126.94999999999999</v>
       </c>
       <c r="C6" s="5">
         <f t="shared" si="1"/>
-        <v>8.7868421052631565</v>
+        <v>6.3474999999999993</v>
       </c>
       <c r="D6">
         <f t="shared" si="2"/>
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E6">
         <v>-5</v>
@@ -1067,22 +1083,25 @@
       <c r="AG6">
         <v>24.75</v>
       </c>
-    </row>
-    <row r="7" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="AH6">
+        <v>-40</v>
+      </c>
+    </row>
+    <row r="7" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B7" s="4">
         <f t="shared" si="0"/>
-        <v>-109.85000000000001</v>
+        <v>-86.65</v>
       </c>
       <c r="C7" s="5">
         <f t="shared" si="1"/>
-        <v>-6.1027777777777779</v>
+        <v>-4.560526315789474</v>
       </c>
       <c r="D7">
         <f t="shared" si="2"/>
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E7">
         <v>-10</v>
@@ -1138,8 +1157,11 @@
       <c r="AG7">
         <v>71.7</v>
       </c>
-    </row>
-    <row r="8" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="AH7">
+        <v>23.2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -1183,7 +1205,7 @@
         <v>20.55</v>
       </c>
     </row>
-    <row r="9" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>17</v>
       </c>
@@ -1221,132 +1243,135 @@
         <v>36.1</v>
       </c>
     </row>
-    <row r="10" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="4">
+        <f t="shared" si="0"/>
+        <v>-37.449999999999996</v>
+      </c>
+      <c r="C10" s="5">
+        <f t="shared" si="1"/>
+        <v>-6.2416666666666663</v>
+      </c>
+      <c r="D10">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+      <c r="E10">
+        <v>-5</v>
+      </c>
+      <c r="J10">
+        <v>-20</v>
+      </c>
+      <c r="L10">
+        <v>33.85</v>
+      </c>
+      <c r="AB10">
+        <v>3.1</v>
+      </c>
+      <c r="AG10">
+        <v>-60</v>
+      </c>
+      <c r="AH10">
+        <v>10.6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>4</v>
       </c>
-      <c r="B10" s="4">
+      <c r="B11" s="4">
         <f t="shared" si="0"/>
         <v>-29.8</v>
       </c>
-      <c r="C10" s="5">
+      <c r="C11" s="5">
         <f t="shared" si="1"/>
         <v>-5.96</v>
       </c>
-      <c r="D10">
+      <c r="D11">
         <f t="shared" si="2"/>
         <v>5</v>
       </c>
-      <c r="E10">
+      <c r="E11">
         <v>11.1</v>
       </c>
-      <c r="F10">
+      <c r="F11">
         <v>-12</v>
       </c>
-      <c r="G10">
+      <c r="G11">
         <v>22.4</v>
       </c>
-      <c r="H10">
+      <c r="H11">
         <v>-40</v>
       </c>
-      <c r="W10">
+      <c r="W11">
         <v>-11.3</v>
       </c>
     </row>
-    <row r="11" spans="1:33" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
+    <row r="12" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="4">
+      <c r="B12" s="4">
         <f t="shared" si="0"/>
         <v>-60.749999999999993</v>
       </c>
-      <c r="C11" s="5">
+      <c r="C12" s="5">
         <f t="shared" si="1"/>
         <v>-12.149999999999999</v>
       </c>
-      <c r="D11">
+      <c r="D12">
         <f t="shared" si="2"/>
         <v>5</v>
       </c>
-      <c r="L11">
+      <c r="L12">
         <v>-8.35</v>
       </c>
-      <c r="M11">
-        <v>-20</v>
-      </c>
-      <c r="P11">
+      <c r="M12">
+        <v>-20</v>
+      </c>
+      <c r="P12">
         <v>-40</v>
       </c>
-      <c r="S11">
+      <c r="S12">
         <v>7.1</v>
       </c>
-      <c r="U11">
+      <c r="U12">
         <v>0.5</v>
       </c>
     </row>
-    <row r="12" spans="1:33" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
+    <row r="13" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>14</v>
       </c>
-      <c r="B12" s="4">
+      <c r="B13" s="4">
         <f t="shared" si="0"/>
         <v>26.500000000000007</v>
       </c>
-      <c r="C12" s="5">
+      <c r="C13" s="5">
         <f t="shared" si="1"/>
         <v>6.6250000000000018</v>
       </c>
-      <c r="D12">
+      <c r="D13">
         <f t="shared" si="2"/>
         <v>4</v>
       </c>
-      <c r="H12">
+      <c r="H13">
         <v>-16.8</v>
       </c>
-      <c r="M12">
+      <c r="M13">
         <v>7.5</v>
       </c>
-      <c r="Q12">
+      <c r="Q13">
         <v>45.7</v>
       </c>
-      <c r="W12">
+      <c r="W13">
         <v>-9.9</v>
       </c>
     </row>
-    <row r="13" spans="1:33" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>9</v>
-      </c>
-      <c r="B13" s="4">
-        <f t="shared" si="0"/>
-        <v>-48.05</v>
-      </c>
-      <c r="C13" s="5">
-        <f t="shared" si="1"/>
-        <v>-9.61</v>
-      </c>
-      <c r="D13">
-        <f t="shared" si="2"/>
-        <v>5</v>
-      </c>
-      <c r="E13">
-        <v>-5</v>
-      </c>
-      <c r="J13">
-        <v>-20</v>
-      </c>
-      <c r="L13">
-        <v>33.85</v>
-      </c>
-      <c r="AB13">
-        <v>3.1</v>
-      </c>
-      <c r="AG13">
-        <v>-60</v>
-      </c>
-    </row>
-    <row r="14" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>16</v>
       </c>
@@ -1375,7 +1400,7 @@
         <v>-30</v>
       </c>
     </row>
-    <row r="15" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>31</v>
       </c>
@@ -1401,7 +1426,7 @@
         <v>51.5</v>
       </c>
     </row>
-    <row r="16" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>13</v>
       </c>
@@ -1427,7 +1452,7 @@
         <v>-4.6500000000000004</v>
       </c>
     </row>
-    <row r="17" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>22</v>
       </c>
@@ -1453,7 +1478,7 @@
         <v>-40</v>
       </c>
     </row>
-    <row r="18" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>20</v>
       </c>
@@ -1476,7 +1501,7 @@
         <v>5.3</v>
       </c>
     </row>
-    <row r="19" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>6</v>
       </c>
@@ -1499,7 +1524,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="20" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>15</v>
       </c>
@@ -1522,7 +1547,7 @@
         <v>-9.1999999999999993</v>
       </c>
     </row>
-    <row r="21" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>24</v>
       </c>
@@ -1545,7 +1570,7 @@
         <v>-30</v>
       </c>
     </row>
-    <row r="22" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>19</v>
       </c>
@@ -1568,7 +1593,7 @@
         <v>-121.7</v>
       </c>
     </row>
-    <row r="23" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>27</v>
       </c>
@@ -1588,7 +1613,7 @@
         <v>76.150000000000006</v>
       </c>
     </row>
-    <row r="24" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>29</v>
       </c>
@@ -1608,7 +1633,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="25" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>33</v>
       </c>
@@ -1628,7 +1653,7 @@
         <v>11.85</v>
       </c>
     </row>
-    <row r="26" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>26</v>
       </c>
@@ -1648,7 +1673,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="27" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>10</v>
       </c>
@@ -1668,7 +1693,7 @@
         <v>-6.35</v>
       </c>
     </row>
-    <row r="28" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>32</v>
       </c>
@@ -1688,7 +1713,7 @@
         <v>-10</v>
       </c>
     </row>
-    <row r="29" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>25</v>
       </c>
@@ -1708,7 +1733,7 @@
         <v>-20</v>
       </c>
     </row>
-    <row r="30" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>23</v>
       </c>
@@ -1728,7 +1753,7 @@
         <v>-20</v>
       </c>
     </row>
-    <row r="31" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>30</v>
       </c>
@@ -1748,7 +1773,7 @@
         <v>-20</v>
       </c>
     </row>
-    <row r="32" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>34</v>
       </c>
@@ -1768,7 +1793,7 @@
         <v>-20</v>
       </c>
     </row>
-    <row r="33" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>28</v>
       </c>
@@ -1788,20 +1813,20 @@
         <v>-30</v>
       </c>
     </row>
-    <row r="34" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>35</v>
       </c>
       <c r="B34" s="4">
-        <f t="shared" ref="B34" si="3">SUM(E34:XFD34)</f>
+        <f t="shared" si="0"/>
         <v>-20</v>
       </c>
       <c r="C34" s="5">
-        <f t="shared" ref="C34" si="4">B34/COUNT(E34:XFD34)</f>
+        <f t="shared" si="1"/>
         <v>-20</v>
       </c>
       <c r="D34">
-        <f t="shared" ref="D34" si="5">COUNT(E34:XFD34)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="AG34">
@@ -1809,10 +1834,10 @@
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:AF33">
-    <sortCondition descending="1" ref="D4:D33"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:AH34">
+    <sortCondition descending="1" ref="D4:D34"/>
   </sortState>
-  <conditionalFormatting sqref="E2:AN7 AL8:AN10 AS8:AZ10 E30:V31 X30:AF31 E11:AN29 E8:AD10 AE9:AF9 E35:AN378 E32:AF34 AG30:AN34 AF8:AG8">
+  <conditionalFormatting sqref="E2:AN7 AL8:AN10 AS8:AZ10 E30:V31 X30:AF31 E11:AN29 E8:AD10 AE9:AF9 E35:AN378 E32:AF34 AG30:AN34 AF8:AG8 AF10:AH10">
     <cfRule type="dataBar" priority="1">
       <dataBar>
         <cfvo type="min"/>
@@ -1826,7 +1851,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:XFD3 E12:O18 Q12:R18 O19 P12:P22 Q20:Q22 E19:F20 M19:N21 R20:R23 E4:R11 T4:XFD7 AL8:XFD10 N22:N27 E21:E27 P23:Q27 S4:S27 T11:XFD18 T8:AD10 AE9:AF9 A2:A34 AF8:AG8">
+  <conditionalFormatting sqref="E2:XFD3 E12:O18 Q12:R18 O19 P12:P22 Q20:Q22 E19:F20 M19:N21 R20:R23 E4:R11 T4:XFD7 AL8:XFD10 N22:N27 E21:E27 P23:Q27 S4:S27 T11:XFD18 T8:AD10 AE9:AF9 A2:A34 AF8:AG8 AF10:AH10">
     <cfRule type="dataBar" priority="4">
       <dataBar>
         <cfvo type="min"/>
@@ -1854,7 +1879,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>E2:AN7 AL8:AN10 AS8:AZ10 E30:V31 X30:AF31 E11:AN29 E8:AD10 AE9:AF9 E35:AN378 E32:AF34 AG30:AN34 AF8:AG8</xm:sqref>
+          <xm:sqref>E2:AN7 AL8:AN10 AS8:AZ10 E30:V31 X30:AF31 E11:AN29 E8:AD10 AE9:AF9 E35:AN378 E32:AF34 AG30:AN34 AF8:AG8 AF10:AH10</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{10B7A0D8-28CC-465F-AF8C-C6786DCEDFCA}">
@@ -1865,7 +1890,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>E2:XFD3 E12:O18 Q12:R18 O19 P12:P22 Q20:Q22 E19:F20 M19:N21 R20:R23 E4:R11 T4:XFD7 AL8:XFD10 N22:N27 E21:E27 P23:Q27 S4:S27 T11:XFD18 T8:AD10 AE9:AF9 A2:A34 AF8:AG8</xm:sqref>
+          <xm:sqref>E2:XFD3 E12:O18 Q12:R18 O19 P12:P22 Q20:Q22 E19:F20 M19:N21 R20:R23 E4:R11 T4:XFD7 AL8:XFD10 N22:N27 E21:E27 P23:Q27 S4:S27 T11:XFD18 T8:AD10 AE9:AF9 A2:A34 AF8:AG8 AF10:AH10</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>

</xml_diff>

<commit_message>
Version 2.1 - Added Games Played to dashboard - 29_11_2023 Data
</commit_message>
<xml_diff>
--- a/Poker League 2023.xlsx
+++ b/Poker League 2023.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PanSt\OneDrive\Υπολογιστής\Poker-League-Game-Analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EFE27B1-96CE-49C0-ACA8-2A57BAD7375C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{377BF246-B78C-4F86-AC32-C589BD20BBD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Φύλλο1" sheetId="1" r:id="rId1"/>
@@ -483,13 +483,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AI34"/>
+  <dimension ref="A1:AJ34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="105" zoomScaleNormal="145" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="M2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="R2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AI2" sqref="AI2"/>
+      <selection pane="bottomRight" activeCell="AG19" sqref="AG19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -498,7 +498,7 @@
     <col min="3" max="3" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:36" x14ac:dyDescent="0.3">
       <c r="B1" s="3" t="s">
         <v>7</v>
       </c>
@@ -601,22 +601,25 @@
       <c r="AI1" s="1">
         <v>45256</v>
       </c>
-    </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="AJ1" s="1">
+        <v>45259</v>
+      </c>
+    </row>
+    <row r="2" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="4">
-        <f t="shared" ref="B2:B34" si="0">SUM(E2:XFD2)</f>
-        <v>80.850000000000009</v>
+        <f>SUM(E2:XFD2)</f>
+        <v>140.60000000000002</v>
       </c>
       <c r="C2" s="5">
-        <f t="shared" ref="C2:C34" si="1">B2/COUNT(E2:XFD2)</f>
-        <v>2.6080645161290326</v>
+        <f>B2/COUNT(E2:XFD2)</f>
+        <v>4.3937500000000007</v>
       </c>
       <c r="D2">
-        <f t="shared" ref="D2:D34" si="2">COUNT(E2:XFD2)</f>
-        <v>31</v>
+        <f>COUNT(E2:XFD2)</f>
+        <v>32</v>
       </c>
       <c r="E2">
         <v>-5</v>
@@ -711,22 +714,25 @@
       <c r="AI2">
         <v>-20</v>
       </c>
-    </row>
-    <row r="3" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="AJ2">
+        <v>59.75</v>
+      </c>
+    </row>
+    <row r="3" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B3" s="4">
-        <f t="shared" si="0"/>
-        <v>88.049999999999983</v>
+        <f>SUM(E3:XFD3)</f>
+        <v>48.049999999999983</v>
       </c>
       <c r="C3" s="5">
-        <f t="shared" si="1"/>
-        <v>3.0362068965517235</v>
+        <f>B3/COUNT(E3:XFD3)</f>
+        <v>1.6016666666666661</v>
       </c>
       <c r="D3">
-        <f t="shared" si="2"/>
-        <v>29</v>
+        <f>COUNT(E3:XFD3)</f>
+        <v>30</v>
       </c>
       <c r="E3">
         <v>-15</v>
@@ -815,22 +821,25 @@
       <c r="AI3">
         <v>-60</v>
       </c>
-    </row>
-    <row r="4" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="AJ3">
+        <v>-40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B4" s="4">
-        <f t="shared" si="0"/>
-        <v>131.41</v>
+        <f>SUM(E4:XFD4)</f>
+        <v>168.61</v>
       </c>
       <c r="C4" s="5">
-        <f t="shared" si="1"/>
-        <v>4.5313793103448274</v>
+        <f>B4/COUNT(E4:XFD4)</f>
+        <v>5.6203333333333338</v>
       </c>
       <c r="D4">
-        <f t="shared" si="2"/>
-        <v>29</v>
+        <f>COUNT(E4:XFD4)</f>
+        <v>30</v>
       </c>
       <c r="E4">
         <v>-0.95</v>
@@ -919,22 +928,25 @@
       <c r="AI4">
         <v>27.6</v>
       </c>
-    </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="AJ4">
+        <v>37.200000000000003</v>
+      </c>
+    </row>
+    <row r="5" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B5" s="4">
-        <f t="shared" si="0"/>
-        <v>44.749999999999986</v>
+        <f>SUM(E5:XFD5)</f>
+        <v>16.599999999999987</v>
       </c>
       <c r="C5" s="5">
-        <f t="shared" si="1"/>
-        <v>1.5431034482758617</v>
+        <f>B5/COUNT(E5:XFD5)</f>
+        <v>0.5533333333333329</v>
       </c>
       <c r="D5">
-        <f t="shared" si="2"/>
-        <v>29</v>
+        <f>COUNT(E5:XFD5)</f>
+        <v>30</v>
       </c>
       <c r="E5">
         <v>37.35</v>
@@ -1023,22 +1035,25 @@
       <c r="AI5">
         <v>-12.95</v>
       </c>
-    </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="AJ5">
+        <v>-28.15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B6" s="4">
-        <f t="shared" si="0"/>
-        <v>142.29999999999998</v>
+        <f>SUM(E6:XFD6)</f>
+        <v>111.29999999999998</v>
       </c>
       <c r="C6" s="5">
-        <f t="shared" si="1"/>
-        <v>6.7761904761904752</v>
+        <f>B6/COUNT(E6:XFD6)</f>
+        <v>5.0590909090909086</v>
       </c>
       <c r="D6">
-        <f t="shared" si="2"/>
-        <v>21</v>
+        <f>COUNT(E6:XFD6)</f>
+        <v>22</v>
       </c>
       <c r="E6">
         <v>-5</v>
@@ -1103,22 +1118,25 @@
       <c r="AI6">
         <v>15.35</v>
       </c>
-    </row>
-    <row r="7" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="AJ6">
+        <v>-31</v>
+      </c>
+    </row>
+    <row r="7" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B7" s="4">
-        <f t="shared" si="0"/>
-        <v>-80.350000000000009</v>
+        <f>SUM(E7:XFD7)</f>
+        <v>-74.2</v>
       </c>
       <c r="C7" s="5">
-        <f t="shared" si="1"/>
-        <v>-4.0175000000000001</v>
+        <f>B7/COUNT(E7:XFD7)</f>
+        <v>-3.5333333333333337</v>
       </c>
       <c r="D7">
-        <f t="shared" si="2"/>
-        <v>20</v>
+        <f>COUNT(E7:XFD7)</f>
+        <v>21</v>
       </c>
       <c r="E7">
         <v>-10</v>
@@ -1180,22 +1198,25 @@
       <c r="AI7">
         <v>6.3</v>
       </c>
-    </row>
-    <row r="8" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="AJ7">
+        <v>6.15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>12</v>
       </c>
       <c r="B8" s="4">
-        <f t="shared" si="0"/>
-        <v>-7.3000000000000007</v>
+        <f>SUM(E8:XFD8)</f>
+        <v>66.350000000000009</v>
       </c>
       <c r="C8" s="5">
-        <f t="shared" si="1"/>
-        <v>-0.81111111111111123</v>
+        <f>B8/COUNT(E8:XFD8)</f>
+        <v>6.6350000000000007</v>
       </c>
       <c r="D8">
-        <f t="shared" si="2"/>
-        <v>9</v>
+        <f>COUNT(E8:XFD8)</f>
+        <v>10</v>
       </c>
       <c r="H8">
         <v>28.2</v>
@@ -1224,97 +1245,103 @@
       <c r="AG8">
         <v>20.55</v>
       </c>
-    </row>
-    <row r="9" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="AJ8">
+        <v>73.650000000000006</v>
+      </c>
+    </row>
+    <row r="9" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="4">
+        <f>SUM(E9:XFD9)</f>
+        <v>-71.349999999999994</v>
+      </c>
+      <c r="C9" s="5">
+        <f>B9/COUNT(E9:XFD9)</f>
+        <v>-8.9187499999999993</v>
+      </c>
+      <c r="D9">
+        <f>COUNT(E9:XFD9)</f>
+        <v>8</v>
+      </c>
+      <c r="E9">
+        <v>-5</v>
+      </c>
+      <c r="J9">
+        <v>-20</v>
+      </c>
+      <c r="L9">
+        <v>33.85</v>
+      </c>
+      <c r="AB9">
+        <v>3.1</v>
+      </c>
+      <c r="AG9">
+        <v>-60</v>
+      </c>
+      <c r="AH9">
+        <v>10.6</v>
+      </c>
+      <c r="AI9">
+        <v>43.7</v>
+      </c>
+      <c r="AJ9">
+        <v>-77.599999999999994</v>
+      </c>
+    </row>
+    <row r="10" spans="1:36" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
         <v>17</v>
       </c>
-      <c r="B9" s="4">
-        <f t="shared" si="0"/>
+      <c r="B10" s="4">
+        <f>SUM(E10:XFD10)</f>
         <v>-93.9</v>
       </c>
-      <c r="C9" s="5">
-        <f t="shared" si="1"/>
+      <c r="C10" s="5">
+        <f>B10/COUNT(E10:XFD10)</f>
         <v>-13.414285714285715</v>
       </c>
-      <c r="D9">
-        <f t="shared" si="2"/>
+      <c r="D10">
+        <f>COUNT(E10:XFD10)</f>
         <v>7</v>
       </c>
-      <c r="L9">
+      <c r="L10">
         <v>-18.95</v>
       </c>
-      <c r="N9">
+      <c r="N10">
         <v>17.399999999999999</v>
       </c>
-      <c r="O9">
+      <c r="O10">
         <v>-40</v>
       </c>
-      <c r="P9">
+      <c r="P10">
         <v>-40</v>
       </c>
-      <c r="AC9">
-        <v>-20</v>
-      </c>
-      <c r="AD9">
+      <c r="AC10">
+        <v>-20</v>
+      </c>
+      <c r="AD10">
         <v>-28.45</v>
       </c>
-      <c r="AF9">
+      <c r="AF10">
         <v>36.1</v>
       </c>
     </row>
-    <row r="10" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>9</v>
-      </c>
-      <c r="B10" s="4">
-        <f t="shared" si="0"/>
-        <v>6.2500000000000071</v>
-      </c>
-      <c r="C10" s="5">
-        <f t="shared" si="1"/>
-        <v>0.8928571428571439</v>
-      </c>
-      <c r="D10">
-        <f t="shared" si="2"/>
-        <v>7</v>
-      </c>
-      <c r="E10">
-        <v>-5</v>
-      </c>
-      <c r="J10">
-        <v>-20</v>
-      </c>
-      <c r="L10">
-        <v>33.85</v>
-      </c>
-      <c r="AB10">
-        <v>3.1</v>
-      </c>
-      <c r="AG10">
-        <v>-60</v>
-      </c>
-      <c r="AH10">
-        <v>10.6</v>
-      </c>
-      <c r="AI10">
-        <v>43.7</v>
-      </c>
-    </row>
-    <row r="11" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>4</v>
       </c>
       <c r="B11" s="4">
-        <f t="shared" si="0"/>
+        <f>SUM(E11:XFD11)</f>
         <v>-29.8</v>
       </c>
       <c r="C11" s="5">
-        <f t="shared" si="1"/>
+        <f>B11/COUNT(E11:XFD11)</f>
         <v>-5.96</v>
       </c>
       <c r="D11">
-        <f t="shared" si="2"/>
+        <f>COUNT(E11:XFD11)</f>
         <v>5</v>
       </c>
       <c r="E11">
@@ -1333,20 +1360,20 @@
         <v>-11.3</v>
       </c>
     </row>
-    <row r="12" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>18</v>
       </c>
       <c r="B12" s="4">
-        <f t="shared" si="0"/>
+        <f>SUM(E12:XFD12)</f>
         <v>-60.749999999999993</v>
       </c>
       <c r="C12" s="5">
-        <f t="shared" si="1"/>
+        <f>B12/COUNT(E12:XFD12)</f>
         <v>-12.149999999999999</v>
       </c>
       <c r="D12">
-        <f t="shared" si="2"/>
+        <f>COUNT(E12:XFD12)</f>
         <v>5</v>
       </c>
       <c r="L12">
@@ -1365,20 +1392,20 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="13" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>14</v>
       </c>
       <c r="B13" s="4">
-        <f t="shared" si="0"/>
+        <f>SUM(E13:XFD13)</f>
         <v>26.500000000000007</v>
       </c>
       <c r="C13" s="5">
-        <f t="shared" si="1"/>
+        <f>B13/COUNT(E13:XFD13)</f>
         <v>6.6250000000000018</v>
       </c>
       <c r="D13">
-        <f t="shared" si="2"/>
+        <f>COUNT(E13:XFD13)</f>
         <v>4</v>
       </c>
       <c r="H13">
@@ -1394,20 +1421,20 @@
         <v>-9.9</v>
       </c>
     </row>
-    <row r="14" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>16</v>
       </c>
       <c r="B14" s="4">
-        <f t="shared" si="0"/>
+        <f>SUM(E14:XFD14)</f>
         <v>-43.85</v>
       </c>
       <c r="C14" s="5">
-        <f t="shared" si="1"/>
+        <f>B14/COUNT(E14:XFD14)</f>
         <v>-10.9625</v>
       </c>
       <c r="D14">
-        <f t="shared" si="2"/>
+        <f>COUNT(E14:XFD14)</f>
         <v>4</v>
       </c>
       <c r="K14">
@@ -1423,20 +1450,20 @@
         <v>-30</v>
       </c>
     </row>
-    <row r="15" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>31</v>
       </c>
       <c r="B15" s="4">
-        <f t="shared" si="0"/>
+        <f>SUM(E15:XFD15)</f>
         <v>24.6</v>
       </c>
       <c r="C15" s="5">
-        <f t="shared" si="1"/>
+        <f>B15/COUNT(E15:XFD15)</f>
         <v>8.2000000000000011</v>
       </c>
       <c r="D15">
-        <f t="shared" si="2"/>
+        <f>COUNT(E15:XFD15)</f>
         <v>3</v>
       </c>
       <c r="X15">
@@ -1449,20 +1476,20 @@
         <v>51.5</v>
       </c>
     </row>
-    <row r="16" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>13</v>
       </c>
       <c r="B16" s="4">
-        <f t="shared" si="0"/>
+        <f>SUM(E16:XFD16)</f>
         <v>16.450000000000003</v>
       </c>
       <c r="C16" s="5">
-        <f t="shared" si="1"/>
+        <f>B16/COUNT(E16:XFD16)</f>
         <v>5.4833333333333343</v>
       </c>
       <c r="D16">
-        <f t="shared" si="2"/>
+        <f>COUNT(E16:XFD16)</f>
         <v>3</v>
       </c>
       <c r="H16">
@@ -1480,15 +1507,15 @@
         <v>22</v>
       </c>
       <c r="B17" s="4">
-        <f t="shared" si="0"/>
+        <f>SUM(E17:XFD17)</f>
         <v>-11.850000000000001</v>
       </c>
       <c r="C17" s="5">
-        <f t="shared" si="1"/>
+        <f>B17/COUNT(E17:XFD17)</f>
         <v>-3.9500000000000006</v>
       </c>
       <c r="D17">
-        <f t="shared" si="2"/>
+        <f>COUNT(E17:XFD17)</f>
         <v>3</v>
       </c>
       <c r="P17">
@@ -1506,15 +1533,15 @@
         <v>20</v>
       </c>
       <c r="B18" s="4">
-        <f t="shared" si="0"/>
+        <f>SUM(E18:XFD18)</f>
         <v>-4.7</v>
       </c>
       <c r="C18" s="5">
-        <f t="shared" si="1"/>
+        <f>B18/COUNT(E18:XFD18)</f>
         <v>-2.35</v>
       </c>
       <c r="D18">
-        <f t="shared" si="2"/>
+        <f>COUNT(E18:XFD18)</f>
         <v>2</v>
       </c>
       <c r="N18">
@@ -1529,15 +1556,15 @@
         <v>6</v>
       </c>
       <c r="B19" s="4">
-        <f t="shared" si="0"/>
+        <f>SUM(E19:XFD19)</f>
         <v>-6.7</v>
       </c>
       <c r="C19" s="5">
-        <f t="shared" si="1"/>
+        <f>B19/COUNT(E19:XFD19)</f>
         <v>-3.35</v>
       </c>
       <c r="D19">
-        <f t="shared" si="2"/>
+        <f>COUNT(E19:XFD19)</f>
         <v>2</v>
       </c>
       <c r="E19">
@@ -1552,15 +1579,15 @@
         <v>15</v>
       </c>
       <c r="B20" s="4">
-        <f t="shared" si="0"/>
+        <f>SUM(E20:XFD20)</f>
         <v>-15.5</v>
       </c>
       <c r="C20" s="5">
-        <f t="shared" si="1"/>
+        <f>B20/COUNT(E20:XFD20)</f>
         <v>-7.75</v>
       </c>
       <c r="D20">
-        <f t="shared" si="2"/>
+        <f>COUNT(E20:XFD20)</f>
         <v>2</v>
       </c>
       <c r="I20">
@@ -1575,15 +1602,15 @@
         <v>24</v>
       </c>
       <c r="B21" s="4">
-        <f t="shared" si="0"/>
+        <f>SUM(E21:XFD21)</f>
         <v>-42.55</v>
       </c>
       <c r="C21" s="5">
-        <f t="shared" si="1"/>
+        <f>B21/COUNT(E21:XFD21)</f>
         <v>-21.274999999999999</v>
       </c>
       <c r="D21">
-        <f t="shared" si="2"/>
+        <f>COUNT(E21:XFD21)</f>
         <v>2</v>
       </c>
       <c r="S21">
@@ -1598,15 +1625,15 @@
         <v>19</v>
       </c>
       <c r="B22" s="4">
-        <f t="shared" si="0"/>
+        <f>SUM(E22:XFD22)</f>
         <v>-157.19999999999999</v>
       </c>
       <c r="C22" s="5">
-        <f t="shared" si="1"/>
+        <f>B22/COUNT(E22:XFD22)</f>
         <v>-78.599999999999994</v>
       </c>
       <c r="D22">
-        <f t="shared" si="2"/>
+        <f>COUNT(E22:XFD22)</f>
         <v>2</v>
       </c>
       <c r="N22">
@@ -1621,15 +1648,15 @@
         <v>27</v>
       </c>
       <c r="B23" s="4">
-        <f t="shared" si="0"/>
+        <f>SUM(E23:XFD23)</f>
         <v>76.150000000000006</v>
       </c>
       <c r="C23" s="5">
-        <f t="shared" si="1"/>
+        <f>B23/COUNT(E23:XFD23)</f>
         <v>76.150000000000006</v>
       </c>
       <c r="D23">
-        <f t="shared" si="2"/>
+        <f>COUNT(E23:XFD23)</f>
         <v>1</v>
       </c>
       <c r="T23">
@@ -1641,15 +1668,15 @@
         <v>29</v>
       </c>
       <c r="B24" s="4">
-        <f t="shared" si="0"/>
+        <f>SUM(E24:XFD24)</f>
         <v>41</v>
       </c>
       <c r="C24" s="5">
-        <f t="shared" si="1"/>
+        <f>B24/COUNT(E24:XFD24)</f>
         <v>41</v>
       </c>
       <c r="D24">
-        <f t="shared" si="2"/>
+        <f>COUNT(E24:XFD24)</f>
         <v>1</v>
       </c>
       <c r="V24">
@@ -1661,15 +1688,15 @@
         <v>33</v>
       </c>
       <c r="B25" s="4">
-        <f t="shared" si="0"/>
+        <f>SUM(E25:XFD25)</f>
         <v>11.85</v>
       </c>
       <c r="C25" s="5">
-        <f t="shared" si="1"/>
+        <f>B25/COUNT(E25:XFD25)</f>
         <v>11.85</v>
       </c>
       <c r="D25">
-        <f t="shared" si="2"/>
+        <f>COUNT(E25:XFD25)</f>
         <v>1</v>
       </c>
       <c r="Z25">
@@ -1681,15 +1708,15 @@
         <v>26</v>
       </c>
       <c r="B26" s="4">
-        <f t="shared" si="0"/>
+        <f>SUM(E26:XFD26)</f>
         <v>11</v>
       </c>
       <c r="C26" s="5">
-        <f t="shared" si="1"/>
+        <f>B26/COUNT(E26:XFD26)</f>
         <v>11</v>
       </c>
       <c r="D26">
-        <f t="shared" si="2"/>
+        <f>COUNT(E26:XFD26)</f>
         <v>1</v>
       </c>
       <c r="T26">
@@ -1701,15 +1728,15 @@
         <v>10</v>
       </c>
       <c r="B27" s="4">
-        <f t="shared" si="0"/>
+        <f>SUM(E27:XFD27)</f>
         <v>-6.35</v>
       </c>
       <c r="C27" s="5">
-        <f t="shared" si="1"/>
+        <f>B27/COUNT(E27:XFD27)</f>
         <v>-6.35</v>
       </c>
       <c r="D27">
-        <f t="shared" si="2"/>
+        <f>COUNT(E27:XFD27)</f>
         <v>1</v>
       </c>
       <c r="F27">
@@ -1721,15 +1748,15 @@
         <v>32</v>
       </c>
       <c r="B28" s="4">
-        <f t="shared" si="0"/>
+        <f>SUM(E28:XFD28)</f>
         <v>-10</v>
       </c>
       <c r="C28" s="5">
-        <f t="shared" si="1"/>
+        <f>B28/COUNT(E28:XFD28)</f>
         <v>-10</v>
       </c>
       <c r="D28">
-        <f t="shared" si="2"/>
+        <f>COUNT(E28:XFD28)</f>
         <v>1</v>
       </c>
       <c r="X28">
@@ -1741,15 +1768,15 @@
         <v>25</v>
       </c>
       <c r="B29" s="4">
-        <f t="shared" si="0"/>
+        <f>SUM(E29:XFD29)</f>
         <v>-20</v>
       </c>
       <c r="C29" s="5">
-        <f t="shared" si="1"/>
+        <f>B29/COUNT(E29:XFD29)</f>
         <v>-20</v>
       </c>
       <c r="D29">
-        <f t="shared" si="2"/>
+        <f>COUNT(E29:XFD29)</f>
         <v>1</v>
       </c>
       <c r="S29">
@@ -1761,15 +1788,15 @@
         <v>23</v>
       </c>
       <c r="B30" s="4">
-        <f t="shared" si="0"/>
+        <f>SUM(E30:XFD30)</f>
         <v>-20</v>
       </c>
       <c r="C30" s="5">
-        <f t="shared" si="1"/>
+        <f>B30/COUNT(E30:XFD30)</f>
         <v>-20</v>
       </c>
       <c r="D30">
-        <f t="shared" si="2"/>
+        <f>COUNT(E30:XFD30)</f>
         <v>1</v>
       </c>
       <c r="Q30">
@@ -1781,15 +1808,15 @@
         <v>30</v>
       </c>
       <c r="B31" s="4">
-        <f t="shared" si="0"/>
+        <f>SUM(E31:XFD31)</f>
         <v>-20</v>
       </c>
       <c r="C31" s="5">
-        <f t="shared" si="1"/>
+        <f>B31/COUNT(E31:XFD31)</f>
         <v>-20</v>
       </c>
       <c r="D31">
-        <f t="shared" si="2"/>
+        <f>COUNT(E31:XFD31)</f>
         <v>1</v>
       </c>
       <c r="V31">
@@ -1801,15 +1828,15 @@
         <v>34</v>
       </c>
       <c r="B32" s="4">
-        <f t="shared" si="0"/>
+        <f>SUM(E32:XFD32)</f>
         <v>-20</v>
       </c>
       <c r="C32" s="5">
-        <f t="shared" si="1"/>
+        <f>B32/COUNT(E32:XFD32)</f>
         <v>-20</v>
       </c>
       <c r="D32">
-        <f t="shared" si="2"/>
+        <f>COUNT(E32:XFD32)</f>
         <v>1</v>
       </c>
       <c r="AC32">
@@ -1821,15 +1848,15 @@
         <v>28</v>
       </c>
       <c r="B33" s="4">
-        <f t="shared" si="0"/>
+        <f>SUM(E33:XFD33)</f>
         <v>-30</v>
       </c>
       <c r="C33" s="5">
-        <f t="shared" si="1"/>
+        <f>B33/COUNT(E33:XFD33)</f>
         <v>-30</v>
       </c>
       <c r="D33">
-        <f t="shared" si="2"/>
+        <f>COUNT(E33:XFD33)</f>
         <v>1</v>
       </c>
       <c r="U33">
@@ -1841,15 +1868,15 @@
         <v>35</v>
       </c>
       <c r="B34" s="4">
-        <f t="shared" si="0"/>
+        <f>SUM(E34:XFD34)</f>
         <v>-20</v>
       </c>
       <c r="C34" s="5">
-        <f t="shared" si="1"/>
+        <f>B34/COUNT(E34:XFD34)</f>
         <v>-20</v>
       </c>
       <c r="D34">
-        <f t="shared" si="2"/>
+        <f>COUNT(E34:XFD34)</f>
         <v>1</v>
       </c>
       <c r="AG34">
@@ -1857,10 +1884,10 @@
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:AH34">
-    <sortCondition descending="1" ref="D4:D34"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:AJ34">
+    <sortCondition descending="1" ref="D3:D34"/>
   </sortState>
-  <conditionalFormatting sqref="E2:AN7 AL8:AN10 AS8:AZ10 E30:V31 X30:AF31 E11:AN29 E8:AD10 AE9:AF9 E35:AN378 E32:AF34 AG30:AN34 AF8:AG8 AF10:AI10">
+  <conditionalFormatting sqref="E2:BG34">
     <cfRule type="dataBar" priority="1">
       <dataBar>
         <cfvo type="min"/>
@@ -1874,7 +1901,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:XFD3 E12:O18 Q12:R18 O19 P12:P22 Q20:Q22 E19:F20 M19:N21 R20:R23 E4:R11 T4:XFD7 AL8:XFD10 N22:N27 E21:E27 P23:Q27 S4:S27 T11:XFD18 T8:AD10 AE9:AF9 A2:A34 AF8:AG8 AF10:AI10">
+  <conditionalFormatting sqref="E2:XFD3 E12:O18 Q12:R18 O19 P12:P22 Q20:Q22 E19:F20 M19:N21 R20:R23 E4:R11 T4:XFD7 AL8:XFD10 N22:N27 E21:E27 P23:Q27 S4:S27 T11:XFD18 T8:AD10 AE9:AF9 A2:A34 AF8:AG8 AJ8 AF10:AJ10">
     <cfRule type="dataBar" priority="4">
       <dataBar>
         <cfvo type="min"/>
@@ -1902,7 +1929,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>E2:AN7 AL8:AN10 AS8:AZ10 E30:V31 X30:AF31 E11:AN29 E8:AD10 AE9:AF9 E35:AN378 E32:AF34 AG30:AN34 AF8:AG8 AF10:AI10</xm:sqref>
+          <xm:sqref>E2:BG34</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{10B7A0D8-28CC-465F-AF8C-C6786DCEDFCA}">
@@ -1913,7 +1940,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>E2:XFD3 E12:O18 Q12:R18 O19 P12:P22 Q20:Q22 E19:F20 M19:N21 R20:R23 E4:R11 T4:XFD7 AL8:XFD10 N22:N27 E21:E27 P23:Q27 S4:S27 T11:XFD18 T8:AD10 AE9:AF9 A2:A34 AF8:AG8 AF10:AI10</xm:sqref>
+          <xm:sqref>E2:XFD3 E12:O18 Q12:R18 O19 P12:P22 Q20:Q22 E19:F20 M19:N21 R20:R23 E4:R11 T4:XFD7 AL8:XFD10 N22:N27 E21:E27 P23:Q27 S4:S27 T11:XFD18 T8:AD10 AE9:AF9 A2:A34 AF8:AG8 AJ8 AF10:AJ10</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>

</xml_diff>

<commit_message>
15_12_2023 data - End of 2023 season
</commit_message>
<xml_diff>
--- a/Poker League 2023.xlsx
+++ b/Poker League 2023.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PanSt\OneDrive\Υπολογιστής\Poker-League-Game-Analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{377BF246-B78C-4F86-AC32-C589BD20BBD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A34BA727-4EB9-4F75-8E3D-B9C3D474A474}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -483,13 +483,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AJ34"/>
+  <dimension ref="A1:AK34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="105" zoomScaleNormal="145" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="R2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="U2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AG19" sqref="AG19"/>
+      <selection pane="bottomRight" activeCell="AH5" sqref="AH5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -498,7 +498,7 @@
     <col min="3" max="3" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:37" x14ac:dyDescent="0.3">
       <c r="B1" s="3" t="s">
         <v>7</v>
       </c>
@@ -604,22 +604,25 @@
       <c r="AJ1" s="1">
         <v>45259</v>
       </c>
-    </row>
-    <row r="2" spans="1:36" x14ac:dyDescent="0.3">
+      <c r="AK1" s="1">
+        <v>45276</v>
+      </c>
+    </row>
+    <row r="2" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="4">
-        <f>SUM(E2:XFD2)</f>
-        <v>140.60000000000002</v>
+        <f t="shared" ref="B2:B34" si="0">SUM(E2:XFD2)</f>
+        <v>269.5</v>
       </c>
       <c r="C2" s="5">
-        <f>B2/COUNT(E2:XFD2)</f>
-        <v>4.3937500000000007</v>
+        <f t="shared" ref="C2:C34" si="1">B2/COUNT(E2:XFD2)</f>
+        <v>8.1666666666666661</v>
       </c>
       <c r="D2">
-        <f>COUNT(E2:XFD2)</f>
-        <v>32</v>
+        <f t="shared" ref="D2:D34" si="2">COUNT(E2:XFD2)</f>
+        <v>33</v>
       </c>
       <c r="E2">
         <v>-5</v>
@@ -717,22 +720,25 @@
       <c r="AJ2">
         <v>59.75</v>
       </c>
-    </row>
-    <row r="3" spans="1:36" x14ac:dyDescent="0.3">
+      <c r="AK2">
+        <v>128.9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B3" s="4">
-        <f>SUM(E3:XFD3)</f>
-        <v>48.049999999999983</v>
+        <f t="shared" si="0"/>
+        <v>57.949999999999982</v>
       </c>
       <c r="C3" s="5">
-        <f>B3/COUNT(E3:XFD3)</f>
-        <v>1.6016666666666661</v>
+        <f t="shared" si="1"/>
+        <v>1.8693548387096768</v>
       </c>
       <c r="D3">
-        <f>COUNT(E3:XFD3)</f>
-        <v>30</v>
+        <f t="shared" si="2"/>
+        <v>31</v>
       </c>
       <c r="E3">
         <v>-15</v>
@@ -824,22 +830,25 @@
       <c r="AJ3">
         <v>-40</v>
       </c>
-    </row>
-    <row r="4" spans="1:36" x14ac:dyDescent="0.3">
+      <c r="AK3">
+        <v>9.9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B4" s="4">
-        <f>SUM(E4:XFD4)</f>
-        <v>168.61</v>
+        <f t="shared" si="0"/>
+        <v>233.20000000000002</v>
       </c>
       <c r="C4" s="5">
-        <f>B4/COUNT(E4:XFD4)</f>
-        <v>5.6203333333333338</v>
+        <f t="shared" si="1"/>
+        <v>7.5225806451612911</v>
       </c>
       <c r="D4">
-        <f>COUNT(E4:XFD4)</f>
-        <v>30</v>
+        <f t="shared" si="2"/>
+        <v>31</v>
       </c>
       <c r="E4">
         <v>-0.95</v>
@@ -923,7 +932,7 @@
         <v>-0.35</v>
       </c>
       <c r="AH4">
-        <v>-5.59</v>
+        <v>-5.6</v>
       </c>
       <c r="AI4">
         <v>27.6</v>
@@ -931,22 +940,25 @@
       <c r="AJ4">
         <v>37.200000000000003</v>
       </c>
-    </row>
-    <row r="5" spans="1:36" x14ac:dyDescent="0.3">
+      <c r="AK4">
+        <v>64.599999999999994</v>
+      </c>
+    </row>
+    <row r="5" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B5" s="4">
-        <f>SUM(E5:XFD5)</f>
-        <v>16.599999999999987</v>
+        <f t="shared" si="0"/>
+        <v>-93.4</v>
       </c>
       <c r="C5" s="5">
-        <f>B5/COUNT(E5:XFD5)</f>
-        <v>0.5533333333333329</v>
+        <f t="shared" si="1"/>
+        <v>-3.0129032258064519</v>
       </c>
       <c r="D5">
-        <f>COUNT(E5:XFD5)</f>
-        <v>30</v>
+        <f t="shared" si="2"/>
+        <v>31</v>
       </c>
       <c r="E5">
         <v>37.35</v>
@@ -1038,22 +1050,25 @@
       <c r="AJ5">
         <v>-28.15</v>
       </c>
-    </row>
-    <row r="6" spans="1:36" x14ac:dyDescent="0.3">
+      <c r="AK5">
+        <v>-110</v>
+      </c>
+    </row>
+    <row r="6" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B6" s="4">
-        <f>SUM(E6:XFD6)</f>
-        <v>111.29999999999998</v>
+        <f t="shared" si="0"/>
+        <v>124.99999999999999</v>
       </c>
       <c r="C6" s="5">
-        <f>B6/COUNT(E6:XFD6)</f>
-        <v>5.0590909090909086</v>
+        <f t="shared" si="1"/>
+        <v>5.4347826086956514</v>
       </c>
       <c r="D6">
-        <f>COUNT(E6:XFD6)</f>
-        <v>22</v>
+        <f t="shared" si="2"/>
+        <v>23</v>
       </c>
       <c r="E6">
         <v>-5</v>
@@ -1121,21 +1136,24 @@
       <c r="AJ6">
         <v>-31</v>
       </c>
-    </row>
-    <row r="7" spans="1:36" x14ac:dyDescent="0.3">
+      <c r="AK6">
+        <v>13.7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B7" s="4">
-        <f>SUM(E7:XFD7)</f>
+        <f t="shared" si="0"/>
         <v>-74.2</v>
       </c>
       <c r="C7" s="5">
-        <f>B7/COUNT(E7:XFD7)</f>
+        <f t="shared" si="1"/>
         <v>-3.5333333333333337</v>
       </c>
       <c r="D7">
-        <f>COUNT(E7:XFD7)</f>
+        <f t="shared" si="2"/>
         <v>21</v>
       </c>
       <c r="E7">
@@ -1202,21 +1220,21 @@
         <v>6.15</v>
       </c>
     </row>
-    <row r="8" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>12</v>
       </c>
       <c r="B8" s="4">
-        <f>SUM(E8:XFD8)</f>
-        <v>66.350000000000009</v>
+        <f t="shared" si="0"/>
+        <v>32.050000000000011</v>
       </c>
       <c r="C8" s="5">
-        <f>B8/COUNT(E8:XFD8)</f>
-        <v>6.6350000000000007</v>
+        <f t="shared" si="1"/>
+        <v>2.9136363636363645</v>
       </c>
       <c r="D8">
-        <f>COUNT(E8:XFD8)</f>
-        <v>10</v>
+        <f t="shared" si="2"/>
+        <v>11</v>
       </c>
       <c r="H8">
         <v>28.2</v>
@@ -1248,22 +1266,25 @@
       <c r="AJ8">
         <v>73.650000000000006</v>
       </c>
-    </row>
-    <row r="9" spans="1:36" x14ac:dyDescent="0.3">
+      <c r="AK8">
+        <v>-34.299999999999997</v>
+      </c>
+    </row>
+    <row r="9" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>9</v>
       </c>
       <c r="B9" s="4">
-        <f>SUM(E9:XFD9)</f>
-        <v>-71.349999999999994</v>
+        <f t="shared" si="0"/>
+        <v>-84.149999999999991</v>
       </c>
       <c r="C9" s="5">
-        <f>B9/COUNT(E9:XFD9)</f>
-        <v>-8.9187499999999993</v>
+        <f t="shared" si="1"/>
+        <v>-9.35</v>
       </c>
       <c r="D9">
-        <f>COUNT(E9:XFD9)</f>
-        <v>8</v>
+        <f t="shared" si="2"/>
+        <v>9</v>
       </c>
       <c r="E9">
         <v>-5</v>
@@ -1289,22 +1310,25 @@
       <c r="AJ9">
         <v>-77.599999999999994</v>
       </c>
-    </row>
-    <row r="10" spans="1:36" x14ac:dyDescent="0.3">
+      <c r="AK9">
+        <v>-12.8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>17</v>
       </c>
       <c r="B10" s="4">
-        <f>SUM(E10:XFD10)</f>
-        <v>-93.9</v>
+        <f t="shared" si="0"/>
+        <v>-153.9</v>
       </c>
       <c r="C10" s="5">
-        <f>B10/COUNT(E10:XFD10)</f>
-        <v>-13.414285714285715</v>
+        <f t="shared" si="1"/>
+        <v>-19.237500000000001</v>
       </c>
       <c r="D10">
-        <f>COUNT(E10:XFD10)</f>
-        <v>7</v>
+        <f t="shared" si="2"/>
+        <v>8</v>
       </c>
       <c r="L10">
         <v>-18.95</v>
@@ -1327,21 +1351,24 @@
       <c r="AF10">
         <v>36.1</v>
       </c>
-    </row>
-    <row r="11" spans="1:36" x14ac:dyDescent="0.3">
+      <c r="AK10">
+        <v>-60</v>
+      </c>
+    </row>
+    <row r="11" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>4</v>
       </c>
       <c r="B11" s="4">
-        <f>SUM(E11:XFD11)</f>
+        <f t="shared" si="0"/>
         <v>-29.8</v>
       </c>
       <c r="C11" s="5">
-        <f>B11/COUNT(E11:XFD11)</f>
+        <f t="shared" si="1"/>
         <v>-5.96</v>
       </c>
       <c r="D11">
-        <f>COUNT(E11:XFD11)</f>
+        <f t="shared" si="2"/>
         <v>5</v>
       </c>
       <c r="E11">
@@ -1360,20 +1387,20 @@
         <v>-11.3</v>
       </c>
     </row>
-    <row r="12" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>18</v>
       </c>
       <c r="B12" s="4">
-        <f>SUM(E12:XFD12)</f>
+        <f t="shared" si="0"/>
         <v>-60.749999999999993</v>
       </c>
       <c r="C12" s="5">
-        <f>B12/COUNT(E12:XFD12)</f>
+        <f t="shared" si="1"/>
         <v>-12.149999999999999</v>
       </c>
       <c r="D12">
-        <f>COUNT(E12:XFD12)</f>
+        <f t="shared" si="2"/>
         <v>5</v>
       </c>
       <c r="L12">
@@ -1392,20 +1419,20 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="13" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>14</v>
       </c>
       <c r="B13" s="4">
-        <f>SUM(E13:XFD13)</f>
+        <f t="shared" si="0"/>
         <v>26.500000000000007</v>
       </c>
       <c r="C13" s="5">
-        <f>B13/COUNT(E13:XFD13)</f>
+        <f t="shared" si="1"/>
         <v>6.6250000000000018</v>
       </c>
       <c r="D13">
-        <f>COUNT(E13:XFD13)</f>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="H13">
@@ -1421,20 +1448,20 @@
         <v>-9.9</v>
       </c>
     </row>
-    <row r="14" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>16</v>
       </c>
       <c r="B14" s="4">
-        <f>SUM(E14:XFD14)</f>
+        <f t="shared" si="0"/>
         <v>-43.85</v>
       </c>
       <c r="C14" s="5">
-        <f>B14/COUNT(E14:XFD14)</f>
+        <f t="shared" si="1"/>
         <v>-10.9625</v>
       </c>
       <c r="D14">
-        <f>COUNT(E14:XFD14)</f>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="K14">
@@ -1450,20 +1477,20 @@
         <v>-30</v>
       </c>
     </row>
-    <row r="15" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>31</v>
       </c>
       <c r="B15" s="4">
-        <f>SUM(E15:XFD15)</f>
+        <f t="shared" si="0"/>
         <v>24.6</v>
       </c>
       <c r="C15" s="5">
-        <f>B15/COUNT(E15:XFD15)</f>
+        <f t="shared" si="1"/>
         <v>8.2000000000000011</v>
       </c>
       <c r="D15">
-        <f>COUNT(E15:XFD15)</f>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="X15">
@@ -1476,20 +1503,20 @@
         <v>51.5</v>
       </c>
     </row>
-    <row r="16" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>13</v>
       </c>
       <c r="B16" s="4">
-        <f>SUM(E16:XFD16)</f>
+        <f t="shared" si="0"/>
         <v>16.450000000000003</v>
       </c>
       <c r="C16" s="5">
-        <f>B16/COUNT(E16:XFD16)</f>
+        <f t="shared" si="1"/>
         <v>5.4833333333333343</v>
       </c>
       <c r="D16">
-        <f>COUNT(E16:XFD16)</f>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="H16">
@@ -1507,15 +1534,15 @@
         <v>22</v>
       </c>
       <c r="B17" s="4">
-        <f>SUM(E17:XFD17)</f>
+        <f t="shared" si="0"/>
         <v>-11.850000000000001</v>
       </c>
       <c r="C17" s="5">
-        <f>B17/COUNT(E17:XFD17)</f>
+        <f t="shared" si="1"/>
         <v>-3.9500000000000006</v>
       </c>
       <c r="D17">
-        <f>COUNT(E17:XFD17)</f>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="P17">
@@ -1533,15 +1560,15 @@
         <v>20</v>
       </c>
       <c r="B18" s="4">
-        <f>SUM(E18:XFD18)</f>
+        <f t="shared" si="0"/>
         <v>-4.7</v>
       </c>
       <c r="C18" s="5">
-        <f>B18/COUNT(E18:XFD18)</f>
+        <f t="shared" si="1"/>
         <v>-2.35</v>
       </c>
       <c r="D18">
-        <f>COUNT(E18:XFD18)</f>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="N18">
@@ -1556,15 +1583,15 @@
         <v>6</v>
       </c>
       <c r="B19" s="4">
-        <f>SUM(E19:XFD19)</f>
+        <f t="shared" si="0"/>
         <v>-6.7</v>
       </c>
       <c r="C19" s="5">
-        <f>B19/COUNT(E19:XFD19)</f>
+        <f t="shared" si="1"/>
         <v>-3.35</v>
       </c>
       <c r="D19">
-        <f>COUNT(E19:XFD19)</f>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="E19">
@@ -1579,15 +1606,15 @@
         <v>15</v>
       </c>
       <c r="B20" s="4">
-        <f>SUM(E20:XFD20)</f>
+        <f t="shared" si="0"/>
         <v>-15.5</v>
       </c>
       <c r="C20" s="5">
-        <f>B20/COUNT(E20:XFD20)</f>
+        <f t="shared" si="1"/>
         <v>-7.75</v>
       </c>
       <c r="D20">
-        <f>COUNT(E20:XFD20)</f>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="I20">
@@ -1602,15 +1629,15 @@
         <v>24</v>
       </c>
       <c r="B21" s="4">
-        <f>SUM(E21:XFD21)</f>
+        <f t="shared" si="0"/>
         <v>-42.55</v>
       </c>
       <c r="C21" s="5">
-        <f>B21/COUNT(E21:XFD21)</f>
+        <f t="shared" si="1"/>
         <v>-21.274999999999999</v>
       </c>
       <c r="D21">
-        <f>COUNT(E21:XFD21)</f>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="S21">
@@ -1625,15 +1652,15 @@
         <v>19</v>
       </c>
       <c r="B22" s="4">
-        <f>SUM(E22:XFD22)</f>
+        <f t="shared" si="0"/>
         <v>-157.19999999999999</v>
       </c>
       <c r="C22" s="5">
-        <f>B22/COUNT(E22:XFD22)</f>
+        <f t="shared" si="1"/>
         <v>-78.599999999999994</v>
       </c>
       <c r="D22">
-        <f>COUNT(E22:XFD22)</f>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="N22">
@@ -1648,15 +1675,15 @@
         <v>27</v>
       </c>
       <c r="B23" s="4">
-        <f>SUM(E23:XFD23)</f>
+        <f t="shared" si="0"/>
         <v>76.150000000000006</v>
       </c>
       <c r="C23" s="5">
-        <f>B23/COUNT(E23:XFD23)</f>
+        <f t="shared" si="1"/>
         <v>76.150000000000006</v>
       </c>
       <c r="D23">
-        <f>COUNT(E23:XFD23)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="T23">
@@ -1668,15 +1695,15 @@
         <v>29</v>
       </c>
       <c r="B24" s="4">
-        <f>SUM(E24:XFD24)</f>
+        <f t="shared" si="0"/>
         <v>41</v>
       </c>
       <c r="C24" s="5">
-        <f>B24/COUNT(E24:XFD24)</f>
+        <f t="shared" si="1"/>
         <v>41</v>
       </c>
       <c r="D24">
-        <f>COUNT(E24:XFD24)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="V24">
@@ -1688,15 +1715,15 @@
         <v>33</v>
       </c>
       <c r="B25" s="4">
-        <f>SUM(E25:XFD25)</f>
+        <f t="shared" si="0"/>
         <v>11.85</v>
       </c>
       <c r="C25" s="5">
-        <f>B25/COUNT(E25:XFD25)</f>
+        <f t="shared" si="1"/>
         <v>11.85</v>
       </c>
       <c r="D25">
-        <f>COUNT(E25:XFD25)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="Z25">
@@ -1708,15 +1735,15 @@
         <v>26</v>
       </c>
       <c r="B26" s="4">
-        <f>SUM(E26:XFD26)</f>
+        <f t="shared" si="0"/>
         <v>11</v>
       </c>
       <c r="C26" s="5">
-        <f>B26/COUNT(E26:XFD26)</f>
+        <f t="shared" si="1"/>
         <v>11</v>
       </c>
       <c r="D26">
-        <f>COUNT(E26:XFD26)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="T26">
@@ -1728,15 +1755,15 @@
         <v>10</v>
       </c>
       <c r="B27" s="4">
-        <f>SUM(E27:XFD27)</f>
+        <f t="shared" si="0"/>
         <v>-6.35</v>
       </c>
       <c r="C27" s="5">
-        <f>B27/COUNT(E27:XFD27)</f>
+        <f t="shared" si="1"/>
         <v>-6.35</v>
       </c>
       <c r="D27">
-        <f>COUNT(E27:XFD27)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="F27">
@@ -1748,15 +1775,15 @@
         <v>32</v>
       </c>
       <c r="B28" s="4">
-        <f>SUM(E28:XFD28)</f>
+        <f t="shared" si="0"/>
         <v>-10</v>
       </c>
       <c r="C28" s="5">
-        <f>B28/COUNT(E28:XFD28)</f>
+        <f t="shared" si="1"/>
         <v>-10</v>
       </c>
       <c r="D28">
-        <f>COUNT(E28:XFD28)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="X28">
@@ -1768,15 +1795,15 @@
         <v>25</v>
       </c>
       <c r="B29" s="4">
-        <f>SUM(E29:XFD29)</f>
+        <f t="shared" si="0"/>
         <v>-20</v>
       </c>
       <c r="C29" s="5">
-        <f>B29/COUNT(E29:XFD29)</f>
+        <f t="shared" si="1"/>
         <v>-20</v>
       </c>
       <c r="D29">
-        <f>COUNT(E29:XFD29)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="S29">
@@ -1788,15 +1815,15 @@
         <v>23</v>
       </c>
       <c r="B30" s="4">
-        <f>SUM(E30:XFD30)</f>
+        <f t="shared" si="0"/>
         <v>-20</v>
       </c>
       <c r="C30" s="5">
-        <f>B30/COUNT(E30:XFD30)</f>
+        <f t="shared" si="1"/>
         <v>-20</v>
       </c>
       <c r="D30">
-        <f>COUNT(E30:XFD30)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="Q30">
@@ -1808,15 +1835,15 @@
         <v>30</v>
       </c>
       <c r="B31" s="4">
-        <f>SUM(E31:XFD31)</f>
+        <f t="shared" si="0"/>
         <v>-20</v>
       </c>
       <c r="C31" s="5">
-        <f>B31/COUNT(E31:XFD31)</f>
+        <f t="shared" si="1"/>
         <v>-20</v>
       </c>
       <c r="D31">
-        <f>COUNT(E31:XFD31)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="V31">
@@ -1828,15 +1855,15 @@
         <v>34</v>
       </c>
       <c r="B32" s="4">
-        <f>SUM(E32:XFD32)</f>
+        <f t="shared" si="0"/>
         <v>-20</v>
       </c>
       <c r="C32" s="5">
-        <f>B32/COUNT(E32:XFD32)</f>
+        <f t="shared" si="1"/>
         <v>-20</v>
       </c>
       <c r="D32">
-        <f>COUNT(E32:XFD32)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="AC32">
@@ -1848,15 +1875,15 @@
         <v>28</v>
       </c>
       <c r="B33" s="4">
-        <f>SUM(E33:XFD33)</f>
+        <f t="shared" si="0"/>
         <v>-30</v>
       </c>
       <c r="C33" s="5">
-        <f>B33/COUNT(E33:XFD33)</f>
+        <f t="shared" si="1"/>
         <v>-30</v>
       </c>
       <c r="D33">
-        <f>COUNT(E33:XFD33)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="U33">
@@ -1868,15 +1895,15 @@
         <v>35</v>
       </c>
       <c r="B34" s="4">
-        <f>SUM(E34:XFD34)</f>
+        <f t="shared" si="0"/>
         <v>-20</v>
       </c>
       <c r="C34" s="5">
-        <f>B34/COUNT(E34:XFD34)</f>
+        <f t="shared" si="1"/>
         <v>-20</v>
       </c>
       <c r="D34">
-        <f>COUNT(E34:XFD34)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="AG34">

</xml_diff>